<commit_message>
Update Excel and CSV user files
</commit_message>
<xml_diff>
--- a/lib/seeds/users.xlsx
+++ b/lib/seeds/users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Documents\smuca\smuca-web\lib\seeds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B20AD9A-F3FC-4E79-B30D-6D4A93B5A114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A644AB6-7EA9-438C-AE19-A965C3DC4A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -375,7 +375,7 @@
       <calculatedColumnFormula>LOWER(SUBSTITUTE(users[[#This Row],[last_name]]," ","_"))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="job_title"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="email" dataDxfId="0">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="email" dataDxfId="1">
       <calculatedColumnFormula>_xlfn.CONCAT(users[[#This Row],[first_name_proper]],".",users[[#This Row],[last_name_proper]],"@", "smuca.fr")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="description"/>
@@ -384,8 +384,8 @@
       <calculatedColumnFormula>_xlfn.CONCAT(users[[#This Row],[first_name_proper]],users[[#This Row],[last_name_proper]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="password_confirmation"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="avatar_filename" dataDxfId="1">
-      <calculatedColumnFormula>_xlfn.CONCAT("avatar","_",users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</calculatedColumnFormula>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="avatar_filename" dataDxfId="0">
+      <calculatedColumnFormula>_xlfn.CONCAT(users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="content_type"/>
   </tableColumns>
@@ -684,7 +684,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -777,8 +777,8 @@
         <v>rachedabassi</v>
       </c>
       <c r="K2" s="3" t="str">
-        <f>_xlfn.CONCAT("avatar","_",users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
-        <v>avatar_rached_abassi.jpeg</v>
+        <f>_xlfn.CONCAT(users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
+        <v>rached_abassi.jpeg</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>15</v>
@@ -821,8 +821,8 @@
         <v>lilaabdelli</v>
       </c>
       <c r="K3" s="3" t="str">
-        <f>_xlfn.CONCAT("avatar","_",users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
-        <v>avatar_lila_abdelli.jpeg</v>
+        <f>_xlfn.CONCAT(users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
+        <v>lila_abdelli.jpeg</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>15</v>
@@ -865,8 +865,8 @@
         <v>fabriceagbemebia</v>
       </c>
       <c r="K4" s="3" t="str">
-        <f>_xlfn.CONCAT("avatar","_",users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
-        <v>avatar_fabrice_agbemebia.jpeg</v>
+        <f>_xlfn.CONCAT(users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
+        <v>fabrice_agbemebia.jpeg</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>15</v>
@@ -909,8 +909,8 @@
         <v>paulandregnette</v>
       </c>
       <c r="K5" s="3" t="str">
-        <f>_xlfn.CONCAT("avatar","_",users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
-        <v>avatar_paul_andregnette.jpeg</v>
+        <f>_xlfn.CONCAT(users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
+        <v>paul_andregnette.jpeg</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>15</v>
@@ -953,8 +953,8 @@
         <v>tarabektache</v>
       </c>
       <c r="K6" s="3" t="str">
-        <f>_xlfn.CONCAT("avatar","_",users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
-        <v>avatar_tara_bektache.jpeg</v>
+        <f>_xlfn.CONCAT(users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
+        <v>tara_bektache.jpeg</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>15</v>
@@ -997,8 +997,8 @@
         <v>alexandrachmelewsky</v>
       </c>
       <c r="K7" s="3" t="str">
-        <f>_xlfn.CONCAT("avatar","_",users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
-        <v>avatar_alexandra_chmelewsky.jpeg</v>
+        <f>_xlfn.CONCAT(users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
+        <v>alexandra_chmelewsky.jpeg</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>15</v>
@@ -1041,8 +1041,8 @@
         <v>tarekdallel</v>
       </c>
       <c r="K8" s="3" t="str">
-        <f>_xlfn.CONCAT("avatar","_",users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
-        <v>avatar_tarek_dallel.jpeg</v>
+        <f>_xlfn.CONCAT(users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
+        <v>tarek_dallel.jpeg</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>15</v>
@@ -1085,8 +1085,8 @@
         <v>frédérickde_ste_mareville</v>
       </c>
       <c r="K9" s="3" t="str">
-        <f>_xlfn.CONCAT("avatar","_",users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
-        <v>avatar_frédérick_de_ste_mareville.jpeg</v>
+        <f>_xlfn.CONCAT(users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
+        <v>frédérick_de_ste_mareville.jpeg</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>15</v>
@@ -1129,8 +1129,8 @@
         <v>hubertdelarue</v>
       </c>
       <c r="K10" s="3" t="str">
-        <f>_xlfn.CONCAT("avatar","_",users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
-        <v>avatar_hubert_delarue.jpeg</v>
+        <f>_xlfn.CONCAT(users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
+        <v>hubert_delarue.jpeg</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>15</v>
@@ -1173,8 +1173,8 @@
         <v>amandinedelassus</v>
       </c>
       <c r="K11" s="3" t="str">
-        <f>_xlfn.CONCAT("avatar","_",users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
-        <v>avatar_amandine_delassus.jpeg</v>
+        <f>_xlfn.CONCAT(users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
+        <v>amandine_delassus.jpeg</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>15</v>
@@ -1217,8 +1217,8 @@
         <v>adriendenis</v>
       </c>
       <c r="K12" s="3" t="str">
-        <f>_xlfn.CONCAT("avatar","_",users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
-        <v>avatar_adrien_denis.jpeg</v>
+        <f>_xlfn.CONCAT(users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
+        <v>adrien_denis.jpeg</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>15</v>
@@ -1261,8 +1261,8 @@
         <v>dimitridesurmont</v>
       </c>
       <c r="K13" s="3" t="str">
-        <f>_xlfn.CONCAT("avatar","_",users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
-        <v>avatar_dimitri_desurmont.jpeg</v>
+        <f>_xlfn.CONCAT(users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
+        <v>dimitri_desurmont.jpeg</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>15</v>
@@ -1305,8 +1305,8 @@
         <v>géraldlorriaux</v>
       </c>
       <c r="K14" s="3" t="str">
-        <f>_xlfn.CONCAT("avatar","_",users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
-        <v>avatar_gérald_lorriaux.jpeg</v>
+        <f>_xlfn.CONCAT(users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
+        <v>gérald_lorriaux.jpeg</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>15</v>
@@ -1349,8 +1349,8 @@
         <v>hacènemoussouni</v>
       </c>
       <c r="K15" s="3" t="str">
-        <f>_xlfn.CONCAT("avatar","_",users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
-        <v>avatar_hacène_moussouni.jpeg</v>
+        <f>_xlfn.CONCAT(users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
+        <v>hacène_moussouni.jpeg</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>15</v>
@@ -1393,8 +1393,8 @@
         <v>antoinepattyn</v>
       </c>
       <c r="K16" s="3" t="str">
-        <f>_xlfn.CONCAT("avatar","_",users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
-        <v>avatar_antoine_pattyn.jpeg</v>
+        <f>_xlfn.CONCAT(users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
+        <v>antoine_pattyn.jpeg</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>15</v>
@@ -1437,8 +1437,8 @@
         <v>sarahpires</v>
       </c>
       <c r="K17" s="3" t="str">
-        <f>_xlfn.CONCAT("avatar","_",users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
-        <v>avatar_sarah_pires.jpeg</v>
+        <f>_xlfn.CONCAT(users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
+        <v>sarah_pires.jpeg</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>15</v>
@@ -1481,8 +1481,8 @@
         <v>frédéricpochet</v>
       </c>
       <c r="K18" s="3" t="str">
-        <f>_xlfn.CONCAT("avatar","_",users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
-        <v>avatar_frédéric_pochet.jpeg</v>
+        <f>_xlfn.CONCAT(users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
+        <v>frédéric_pochet.jpeg</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>15</v>
@@ -1525,8 +1525,8 @@
         <v>corinnepotin</v>
       </c>
       <c r="K19" s="3" t="str">
-        <f>_xlfn.CONCAT("avatar","_",users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
-        <v>avatar_corinne_potin.jpeg</v>
+        <f>_xlfn.CONCAT(users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
+        <v>corinne_potin.jpeg</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>15</v>
@@ -1569,8 +1569,8 @@
         <v>khalidregany</v>
       </c>
       <c r="K20" s="3" t="str">
-        <f>_xlfn.CONCAT("avatar","_",users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
-        <v>avatar_khalid_regany.jpeg</v>
+        <f>_xlfn.CONCAT(users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
+        <v>khalid_regany.jpeg</v>
       </c>
       <c r="L20" s="1" t="s">
         <v>15</v>
@@ -1613,8 +1613,8 @@
         <v>matthiassabrachou</v>
       </c>
       <c r="K21" s="3" t="str">
-        <f>_xlfn.CONCAT("avatar","_",users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
-        <v>avatar_matthias_sabrachou.jpeg</v>
+        <f>_xlfn.CONCAT(users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
+        <v>matthias_sabrachou.jpeg</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>15</v>
@@ -1657,8 +1657,8 @@
         <v>chloéspriet</v>
       </c>
       <c r="K22" s="3" t="str">
-        <f>_xlfn.CONCAT("avatar","_",users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
-        <v>avatar_chloé_spriet.jpeg</v>
+        <f>_xlfn.CONCAT(users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
+        <v>chloé_spriet.jpeg</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>15</v>
@@ -1701,8 +1701,8 @@
         <v>laurenturso</v>
       </c>
       <c r="K23" s="3" t="str">
-        <f>_xlfn.CONCAT("avatar","_",users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
-        <v>avatar_laurent_urso.jpeg</v>
+        <f>_xlfn.CONCAT(users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
+        <v>laurent_urso.jpeg</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Add website admin user to Excel files
</commit_message>
<xml_diff>
--- a/lib/seeds/users.xlsx
+++ b/lib/seeds/users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Documents\smuca\smuca-web\lib\seeds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF933C41-A75E-4A36-86FF-80D0A24AB804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0589F12B-15D1-4685-A766-0B9531F4533C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="88">
   <si>
     <t>first_name</t>
   </si>
@@ -284,6 +284,18 @@
   </si>
   <si>
     <t>Médecin associée</t>
+  </si>
+  <si>
+    <t>Super</t>
+  </si>
+  <si>
+    <t>ADMIN</t>
+  </si>
+  <si>
+    <t>Website administrator</t>
+  </si>
+  <si>
+    <t>+33 0 00 00 00 00</t>
   </si>
 </sst>
 </file>
@@ -319,11 +331,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -357,8 +371,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="users" displayName="users" ref="A1:L23" totalsRowShown="0">
-  <autoFilter ref="A1:L23" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="users" displayName="users" ref="A1:L24" totalsRowShown="0">
+  <autoFilter ref="A1:L24" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="first_name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="last_name"/>
@@ -675,10 +689,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="C18" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1702,6 +1716,50 @@
         <v>14</v>
       </c>
     </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A24" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="3" t="str">
+        <f>LOWER(SUBSTITUTE(users[[#This Row],[first_name]]," ","_"))</f>
+        <v>super</v>
+      </c>
+      <c r="D24" s="4" t="str">
+        <f>LOWER(SUBSTITUTE(users[[#This Row],[last_name]]," ","_"))</f>
+        <v>admin</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F24" s="4" t="str">
+        <f>_xlfn.CONCAT(users[[#This Row],[first_name_proper]],".",users[[#This Row],[last_name_proper]],"@", "smuca.fr")</f>
+        <v>super.admin@smuca.fr</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="I24" s="3" t="str">
+        <f>_xlfn.CONCAT(users[[#This Row],[first_name_proper]],users[[#This Row],[last_name_proper]])</f>
+        <v>superadmin</v>
+      </c>
+      <c r="J24" s="3" t="str">
+        <f>users[[#This Row], [password]]</f>
+        <v>superadmin</v>
+      </c>
+      <c r="K24" s="4" t="str">
+        <f>_xlfn.CONCAT(users[[#This Row],[first_name_proper]],"_",users[[#This Row],[last_name_proper]],".jpeg")</f>
+        <v>super_admin.jpeg</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>